<commit_message>
added comments in code
</commit_message>
<xml_diff>
--- a/cointegration_results.xlsx
+++ b/cointegration_results.xlsx
@@ -502,13 +502,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.618394969665232</v>
+        <v>0.6183949840649011</v>
       </c>
       <c r="E2" t="n">
-        <v>0.000781980583406461</v>
+        <v>0.0007819938653903547</v>
       </c>
       <c r="F2" t="n">
-        <v>24.96721089450704</v>
+        <v>24.96723852706736</v>
       </c>
       <c r="G2" t="n">
         <v>15.4943</v>
@@ -517,11 +517,11 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>1.611380371782336</v>
+        <v>1.611382155183994</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[ 0.31778084 -0.06268571]</t>
+          <t>[ 0.31778081 -0.06268569]</t>
         </is>
       </c>
     </row>
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.6325630226261103</v>
+        <v>0.6325630073287644</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01836911944470726</v>
+        <v>0.01836905748085003</v>
       </c>
       <c r="F3" t="n">
-        <v>16.73686147930997</v>
+        <v>16.73684346747135</v>
       </c>
       <c r="G3" t="n">
         <v>15.4943</v>
@@ -557,11 +557,11 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>1.080194747701411</v>
+        <v>1.080193585219813</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[0.17631907 0.04110179]</t>
+          <t>[0.17631894 0.04110196]</t>
         </is>
       </c>
     </row>
@@ -582,13 +582,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.7024687305701155</v>
+        <v>0.7024686787693805</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3814596230032011</v>
+        <v>0.381460095988693</v>
       </c>
       <c r="F4" t="n">
-        <v>9.977905992295254</v>
+        <v>9.977877839429048</v>
       </c>
       <c r="G4" t="n">
         <v>15.4943</v>
@@ -597,11 +597,11 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6439726862326954</v>
+        <v>0.6439708692505662</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[0.02421943 0.12041567]</t>
+          <t>[0.02421957 0.12041545]</t>
         </is>
       </c>
     </row>
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.6035279342161003</v>
+        <v>0.6035278543255299</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0006166695106920629</v>
+        <v>0.0006166652298220817</v>
       </c>
       <c r="F5" t="n">
-        <v>20.22049909820509</v>
+        <v>20.22051492922491</v>
       </c>
       <c r="G5" t="n">
         <v>15.4943</v>
@@ -637,11 +637,11 @@
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>1.305028242528226</v>
+        <v>1.305029264260077</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>[ 0.19538447 -0.25052377]</t>
+          <t>[ 0.19538445 -0.25052375]</t>
         </is>
       </c>
     </row>
@@ -662,13 +662,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.6754184116864532</v>
+        <v>0.6754184082610786</v>
       </c>
       <c r="E6" t="n">
-        <v>0.002798437051923906</v>
+        <v>0.002798446101486107</v>
       </c>
       <c r="F6" t="n">
-        <v>18.89070871721745</v>
+        <v>18.89073830814724</v>
       </c>
       <c r="G6" t="n">
         <v>15.4943</v>
@@ -677,11 +677,11 @@
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>1.219203753458849</v>
+        <v>1.219205663253405</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[ 0.13661116 -0.35028055]</t>
+          <t>[ 0.13661119 -0.35028069]</t>
         </is>
       </c>
     </row>
@@ -702,13 +702,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.8712663803313752</v>
+        <v>0.8712663639086411</v>
       </c>
       <c r="E7" t="n">
-        <v>0.001267736030705901</v>
+        <v>0.001267735632991838</v>
       </c>
       <c r="F7" t="n">
-        <v>18.60605012052827</v>
+        <v>18.6060452984982</v>
       </c>
       <c r="G7" t="n">
         <v>15.4943</v>
@@ -717,11 +717,11 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>1.200831926613546</v>
+        <v>1.200831615400386</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[ 0.4358811  -0.54375425]</t>
+          <t>[ 0.43588107 -0.54375418]</t>
         </is>
       </c>
     </row>
@@ -742,13 +742,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.8480505734461893</v>
+        <v>0.8480505866909828</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01197735206776944</v>
+        <v>0.01197726617947072</v>
       </c>
       <c r="F8" t="n">
-        <v>16.00554439284594</v>
+        <v>16.00553066823936</v>
       </c>
       <c r="G8" t="n">
         <v>15.4943</v>
@@ -757,11 +757,11 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>1.032995643097522</v>
+        <v>1.032994757313293</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[ 0.37952503 -0.46381191]</t>
+          <t>[ 0.37952501 -0.46381186]</t>
         </is>
       </c>
     </row>
@@ -782,13 +782,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.7302709612063399</v>
+        <v>0.7302709556458745</v>
       </c>
       <c r="E9" t="n">
-        <v>0.009544960583373551</v>
+        <v>0.009545117298338521</v>
       </c>
       <c r="F9" t="n">
-        <v>15.67205433667856</v>
+        <v>15.67207148204413</v>
       </c>
       <c r="G9" t="n">
         <v>15.4943</v>
@@ -797,11 +797,11 @@
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>1.01147224054514</v>
+        <v>1.011473347104686</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>[ 0.37999039 -0.04464736]</t>
+          <t>[ 0.37999037 -0.04464737]</t>
         </is>
       </c>
     </row>
@@ -822,13 +822,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.7964449857897462</v>
+        <v>0.7964449650503628</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02341066919750473</v>
+        <v>0.0234106584591638</v>
       </c>
       <c r="F10" t="n">
-        <v>10.45987761795412</v>
+        <v>10.45987912316099</v>
       </c>
       <c r="G10" t="n">
         <v>15.4943</v>
@@ -837,11 +837,11 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6750790689449748</v>
+        <v>0.6750791660908199</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>[ 0.40515238 -0.38743097]</t>
+          <t>[ 0.40515237 -0.38743099]</t>
         </is>
       </c>
     </row>
@@ -862,13 +862,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.7386033608676056</v>
+        <v>0.7386033235556743</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01826055452387614</v>
+        <v>0.01826057667263337</v>
       </c>
       <c r="F11" t="n">
-        <v>12.30913075290531</v>
+        <v>12.30911419801227</v>
       </c>
       <c r="G11" t="n">
         <v>15.4943</v>
@@ -877,11 +877,11 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.7944296130128701</v>
+        <v>0.7944285445623402</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>[ 0.41547964 -0.03906522]</t>
+          <t>[ 0.4154796  -0.03906522]</t>
         </is>
       </c>
     </row>
@@ -902,13 +902,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.778242971174568</v>
+        <v>0.7782429767873497</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02953499712334373</v>
+        <v>0.02953494372728297</v>
       </c>
       <c r="F12" t="n">
-        <v>10.78441589730852</v>
+        <v>10.78442102754372</v>
       </c>
       <c r="G12" t="n">
         <v>15.4943</v>
@@ -917,11 +917,11 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6960247250478255</v>
+        <v>0.6960250561525023</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>[ 0.33661073 -0.03340498]</t>
+          <t>[ 0.33661067 -0.03340498]</t>
         </is>
       </c>
     </row>
@@ -942,13 +942,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.7515368365878226</v>
+        <v>0.751536855936819</v>
       </c>
       <c r="E13" t="n">
-        <v>0.01912826641087483</v>
+        <v>0.01912854279031435</v>
       </c>
       <c r="F13" t="n">
-        <v>18.37783241081517</v>
+        <v>18.3778024683985</v>
       </c>
       <c r="G13" t="n">
         <v>15.4943</v>
@@ -957,11 +957,11 @@
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>1.186102786883897</v>
+        <v>1.186100854404426</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>[ 0.21263175 -0.31504718]</t>
+          <t>[ 0.2126317  -0.31504718]</t>
         </is>
       </c>
     </row>
@@ -982,13 +982,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.772185266197415</v>
+        <v>0.7721853018678833</v>
       </c>
       <c r="E14" t="n">
-        <v>0.03016451238756879</v>
+        <v>0.03016477551485748</v>
       </c>
       <c r="F14" t="n">
-        <v>9.293371438736573</v>
+        <v>9.293356106216711</v>
       </c>
       <c r="G14" t="n">
         <v>15.4943</v>
@@ -997,11 +997,11 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>0.5997929198954823</v>
+        <v>0.5997919303367504</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>[ 0.26785422 -0.09700595]</t>
+          <t>[ 0.26785419 -0.09700595]</t>
         </is>
       </c>
     </row>
@@ -1022,13 +1022,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.5505465708131623</v>
+        <v>0.5505465875505141</v>
       </c>
       <c r="E15" t="n">
-        <v>0.06868492905050502</v>
+        <v>0.0686855988563593</v>
       </c>
       <c r="F15" t="n">
-        <v>7.381520279563269</v>
+        <v>7.381506096692615</v>
       </c>
       <c r="G15" t="n">
         <v>15.4943</v>
@@ -1037,11 +1037,11 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0.4764023079173159</v>
+        <v>0.4764013925567863</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>[ 0.21649301 -0.02877683]</t>
+          <t>[ 0.21649302 -0.02877683]</t>
         </is>
       </c>
     </row>
@@ -1062,13 +1062,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.6020397632573915</v>
+        <v>0.6020398630407148</v>
       </c>
       <c r="E16" t="n">
-        <v>0.06314376245048041</v>
+        <v>0.0631437496157131</v>
       </c>
       <c r="F16" t="n">
-        <v>8.524169713459859</v>
+        <v>8.524155079169752</v>
       </c>
       <c r="G16" t="n">
         <v>15.4943</v>
@@ -1077,11 +1077,11 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.5501487458910604</v>
+        <v>0.5501478013959812</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>[ 0.22800413 -0.0513753 ]</t>
+          <t>[ 0.22800415 -0.05137533]</t>
         </is>
       </c>
     </row>
@@ -1102,13 +1102,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.3725246233334805</v>
+        <v>0.3725246422785028</v>
       </c>
       <c r="E17" t="n">
-        <v>0.08313854276216132</v>
+        <v>0.08313837459882889</v>
       </c>
       <c r="F17" t="n">
-        <v>7.31971590997417</v>
+        <v>7.319725762113397</v>
       </c>
       <c r="G17" t="n">
         <v>15.4943</v>
@@ -1117,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>0.4724134623683658</v>
+        <v>0.4724140982240822</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1142,13 +1142,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.7658830701543439</v>
+        <v>0.7658830705050073</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01911854022244503</v>
+        <v>0.01911828951625773</v>
       </c>
       <c r="F18" t="n">
-        <v>15.74101557711128</v>
+        <v>15.74095588352838</v>
       </c>
       <c r="G18" t="n">
         <v>15.4943</v>
@@ -1157,7 +1157,7 @@
         <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>1.015922989558178</v>
+        <v>1.015919136942513</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1182,13 +1182,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.602138622903305</v>
+        <v>0.6021386179596223</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0008485784873502389</v>
+        <v>0.0008485689004768245</v>
       </c>
       <c r="F19" t="n">
-        <v>18.15956139826049</v>
+        <v>18.15947727430979</v>
       </c>
       <c r="G19" t="n">
         <v>15.4943</v>
@@ -1197,11 +1197,11 @@
         <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>1.172015605626617</v>
+        <v>1.17201017627836</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>[ 0.55961215 -0.06370079]</t>
+          <t>[ 0.55961217 -0.06370079]</t>
         </is>
       </c>
     </row>
@@ -1222,13 +1222,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.6099209510046056</v>
+        <v>0.6099211632949364</v>
       </c>
       <c r="E20" t="n">
-        <v>0.002027428914242832</v>
+        <v>0.002027452177843329</v>
       </c>
       <c r="F20" t="n">
-        <v>17.59095242460737</v>
+        <v>17.59091876843787</v>
       </c>
       <c r="G20" t="n">
         <v>15.4943</v>
@@ -1237,11 +1237,11 @@
         <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>1.135317660340084</v>
+        <v>1.135315488175514</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>[ 0.47875295 -0.20064186]</t>
+          <t>[ 0.47875303 -0.20064189]</t>
         </is>
       </c>
     </row>
@@ -1262,13 +1262,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.4275100720734901</v>
+        <v>0.4275101408568411</v>
       </c>
       <c r="E21" t="n">
-        <v>0.03383101591907973</v>
+        <v>0.03383156531121734</v>
       </c>
       <c r="F21" t="n">
-        <v>10.48520240821987</v>
+        <v>10.48519306123329</v>
       </c>
       <c r="G21" t="n">
         <v>15.4943</v>
@@ -1277,11 +1277,11 @@
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0.6767135274404054</v>
+        <v>0.6767129241871717</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>[ 0.36061118 -0.50433339]</t>
+          <t>[ 0.36061123 -0.50433333]</t>
         </is>
       </c>
     </row>
@@ -1302,13 +1302,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.5978224627098094</v>
+        <v>0.5978225160495485</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01126708230409281</v>
+        <v>0.01126702359254859</v>
       </c>
       <c r="F22" t="n">
-        <v>12.38659903806067</v>
+        <v>12.38660744062619</v>
       </c>
       <c r="G22" t="n">
         <v>15.4943</v>
@@ -1317,11 +1317,11 @@
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>0.7994294055272368</v>
+        <v>0.799429947827665</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>[ 0.47100361 -0.18720612]</t>
+          <t>[ 0.4710037  -0.18720619]</t>
         </is>
       </c>
     </row>
@@ -1342,13 +1342,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.626929027215725</v>
+        <v>0.6269288243491759</v>
       </c>
       <c r="E23" t="n">
-        <v>0.275003022021716</v>
+        <v>0.2750023459548397</v>
       </c>
       <c r="F23" t="n">
-        <v>7.09765896141852</v>
+        <v>7.097655564617231</v>
       </c>
       <c r="G23" t="n">
         <v>15.4943</v>
@@ -1357,11 +1357,11 @@
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0.4580819373200802</v>
+        <v>0.4580817180909902</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>[ 0.12747956 -0.40589621]</t>
+          <t>[ 0.12747955 -0.40589609]</t>
         </is>
       </c>
     </row>
@@ -1382,13 +1382,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.6420917458156249</v>
+        <v>0.6420917582793985</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1013522965056777</v>
+        <v>0.1013521746878666</v>
       </c>
       <c r="F24" t="n">
-        <v>7.818911617268935</v>
+        <v>7.81891255800633</v>
       </c>
       <c r="G24" t="n">
         <v>15.4943</v>
@@ -1397,11 +1397,11 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>0.5046314849505259</v>
+        <v>0.5046315456655887</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>[ 0.14088653 -0.12248267]</t>
+          <t>[ 0.1408865  -0.12248264]</t>
         </is>
       </c>
     </row>
@@ -1422,13 +1422,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.6850898797042853</v>
+        <v>0.6850898890537228</v>
       </c>
       <c r="E25" t="n">
-        <v>0.001150549317379958</v>
+        <v>0.001150513855321031</v>
       </c>
       <c r="F25" t="n">
-        <v>16.78219470962773</v>
+        <v>16.78220018378531</v>
       </c>
       <c r="G25" t="n">
         <v>15.4943</v>
@@ -1437,11 +1437,11 @@
         <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>1.083120548177571</v>
+        <v>1.083120901478951</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>[ 0.76322759 -0.22079368]</t>
+          <t>[ 0.7632276  -0.22079367]</t>
         </is>
       </c>
     </row>
@@ -1462,13 +1462,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.7037610201477942</v>
+        <v>0.703761072875736</v>
       </c>
       <c r="E26" t="n">
-        <v>0.002482819041561035</v>
+        <v>0.002482864907776305</v>
       </c>
       <c r="F26" t="n">
-        <v>17.44926338383751</v>
+        <v>17.44921113920149</v>
       </c>
       <c r="G26" t="n">
         <v>15.4943</v>
@@ -1477,11 +1477,11 @@
         <v>1</v>
       </c>
       <c r="I26" t="n">
-        <v>1.12617306905362</v>
+        <v>1.126169697191967</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>[ 0.60993775 -0.71030691]</t>
+          <t>[ 0.60993769 -0.71030695]</t>
         </is>
       </c>
     </row>
@@ -1502,13 +1502,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.6463059478171461</v>
+        <v>0.6463059403572415</v>
       </c>
       <c r="E27" t="n">
-        <v>0.003637001407434561</v>
+        <v>0.003636998589662188</v>
       </c>
       <c r="F27" t="n">
-        <v>15.61975465934927</v>
+        <v>15.61973390592196</v>
       </c>
       <c r="G27" t="n">
         <v>15.4943</v>
@@ -1517,11 +1517,11 @@
         <v>1</v>
       </c>
       <c r="I27" t="n">
-        <v>1.008096826532936</v>
+        <v>1.00809548710958</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>[ 0.26978575 -0.07183855]</t>
+          <t>[ 0.26978576 -0.07183855]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
plot and minor changes
</commit_message>
<xml_diff>
--- a/cointegration_results.xlsx
+++ b/cointegration_results.xlsx
@@ -502,13 +502,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.6183949840649011</v>
+        <v>0.6183950451608057</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0007819938653903547</v>
+        <v>0.0007819828803196954</v>
       </c>
       <c r="F2" t="n">
-        <v>24.96723852706736</v>
+        <v>24.96723176342669</v>
       </c>
       <c r="G2" t="n">
         <v>15.4943</v>
@@ -517,11 +517,11 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>1.611382155183994</v>
+        <v>1.611381718659552</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[ 0.31778081 -0.06268569]</t>
+          <t>[ 0.31778082 -0.06268567]</t>
         </is>
       </c>
     </row>
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.6325630073287644</v>
+        <v>0.6325629441036188</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01836905748085003</v>
+        <v>0.01836892643032831</v>
       </c>
       <c r="F3" t="n">
-        <v>16.73684346747135</v>
+        <v>16.73684223409452</v>
       </c>
       <c r="G3" t="n">
         <v>15.4943</v>
@@ -557,11 +557,11 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>1.080193585219813</v>
+        <v>1.080193505617841</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[0.17631894 0.04110196]</t>
+          <t>[0.176319   0.04110187]</t>
         </is>
       </c>
     </row>
@@ -582,13 +582,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.7024686787693805</v>
+        <v>0.7024686972505991</v>
       </c>
       <c r="E4" t="n">
-        <v>0.381460095988693</v>
+        <v>0.3814594999279021</v>
       </c>
       <c r="F4" t="n">
-        <v>9.977877839429048</v>
+        <v>9.977897272211113</v>
       </c>
       <c r="G4" t="n">
         <v>15.4943</v>
@@ -597,11 +597,11 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6439708692505662</v>
+        <v>0.6439721234396593</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[0.02421957 0.12041545]</t>
+          <t>[0.02421953 0.12041552]</t>
         </is>
       </c>
     </row>
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.6035278543255299</v>
+        <v>0.6035278586660175</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0006166652298220817</v>
+        <v>0.0006166715590086611</v>
       </c>
       <c r="F5" t="n">
-        <v>20.22051492922491</v>
+        <v>20.22047146842954</v>
       </c>
       <c r="G5" t="n">
         <v>15.4943</v>
@@ -637,11 +637,11 @@
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>1.305029264260077</v>
+        <v>1.305026459306296</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>[ 0.19538445 -0.25052375]</t>
+          <t>[ 0.19538445 -0.25052374]</t>
         </is>
       </c>
     </row>
@@ -662,13 +662,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.6754184082610786</v>
+        <v>0.675418437646664</v>
       </c>
       <c r="E6" t="n">
-        <v>0.002798446101486107</v>
+        <v>0.002798440864392866</v>
       </c>
       <c r="F6" t="n">
-        <v>18.89073830814724</v>
+        <v>18.89071872877038</v>
       </c>
       <c r="G6" t="n">
         <v>15.4943</v>
@@ -677,11 +677,11 @@
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>1.219205663253405</v>
+        <v>1.219204399603104</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[ 0.13661119 -0.35028069]</t>
+          <t>[ 0.13661115 -0.3502805 ]</t>
         </is>
       </c>
     </row>
@@ -702,13 +702,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.8712663639086411</v>
+        <v>0.8712663961374646</v>
       </c>
       <c r="E7" t="n">
-        <v>0.001267735632991838</v>
+        <v>0.001267772930683297</v>
       </c>
       <c r="F7" t="n">
-        <v>18.6060452984982</v>
+        <v>18.6059829129727</v>
       </c>
       <c r="G7" t="n">
         <v>15.4943</v>
@@ -717,11 +717,11 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>1.200831615400386</v>
+        <v>1.200827589047114</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[ 0.43588107 -0.54375418]</t>
+          <t>[ 0.43588112 -0.54375427]</t>
         </is>
       </c>
     </row>
@@ -742,13 +742,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.8480505866909828</v>
+        <v>0.8480506102993624</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01197726617947072</v>
+        <v>0.01197733081141318</v>
       </c>
       <c r="F8" t="n">
-        <v>16.00553066823936</v>
+        <v>16.0055076266447</v>
       </c>
       <c r="G8" t="n">
         <v>15.4943</v>
@@ -757,11 +757,11 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>1.032994757313293</v>
+        <v>1.03299327021193</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[ 0.37952501 -0.46381186]</t>
+          <t>[ 0.37952504 -0.46381184]</t>
         </is>
       </c>
     </row>
@@ -782,13 +782,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.7302709556458745</v>
+        <v>0.7302709731347655</v>
       </c>
       <c r="E9" t="n">
-        <v>0.009545117298338521</v>
+        <v>0.00954509154990923</v>
       </c>
       <c r="F9" t="n">
-        <v>15.67207148204413</v>
+        <v>15.67207963345827</v>
       </c>
       <c r="G9" t="n">
         <v>15.4943</v>
@@ -797,11 +797,11 @@
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>1.011473347104686</v>
+        <v>1.011473873195838</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>[ 0.37999037 -0.04464737]</t>
+          <t>[ 0.37999036 -0.04464736]</t>
         </is>
       </c>
     </row>
@@ -822,13 +822,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.7964449650503628</v>
+        <v>0.7964450256248707</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0234106584591638</v>
+        <v>0.02341053620396535</v>
       </c>
       <c r="F10" t="n">
-        <v>10.45987912316099</v>
+        <v>10.45988880418429</v>
       </c>
       <c r="G10" t="n">
         <v>15.4943</v>
@@ -837,11 +837,11 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6750791660908199</v>
+        <v>0.6750797909027378</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>[ 0.40515237 -0.38743099]</t>
+          <t>[ 0.40515241 -0.3874311 ]</t>
         </is>
       </c>
     </row>
@@ -862,13 +862,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.7386033235556743</v>
+        <v>0.7386033464125396</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01826057667263337</v>
+        <v>0.01826050842569454</v>
       </c>
       <c r="F11" t="n">
-        <v>12.30911419801227</v>
+        <v>12.30909841830705</v>
       </c>
       <c r="G11" t="n">
         <v>15.4943</v>
@@ -877,11 +877,11 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.7944285445623402</v>
+        <v>0.7944275261423266</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>[ 0.4154796  -0.03906522]</t>
+          <t>[ 0.41547965 -0.03906522]</t>
         </is>
       </c>
     </row>
@@ -902,13 +902,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.7782429767873497</v>
+        <v>0.7782430363992037</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02953494372728297</v>
+        <v>0.0295349030511869</v>
       </c>
       <c r="F12" t="n">
-        <v>10.78442102754372</v>
+        <v>10.78444352841938</v>
       </c>
       <c r="G12" t="n">
         <v>15.4943</v>
@@ -917,11 +917,11 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6960250561525023</v>
+        <v>0.6960265083559363</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>[ 0.33661067 -0.03340498]</t>
+          <t>[ 0.33661073 -0.03340498]</t>
         </is>
       </c>
     </row>
@@ -942,13 +942,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.751536855936819</v>
+        <v>0.7515369188484933</v>
       </c>
       <c r="E13" t="n">
-        <v>0.01912854279031435</v>
+        <v>0.01912841741346826</v>
       </c>
       <c r="F13" t="n">
-        <v>18.3778024683985</v>
+        <v>18.37780103456878</v>
       </c>
       <c r="G13" t="n">
         <v>15.4943</v>
@@ -957,11 +957,11 @@
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>1.186100854404426</v>
+        <v>1.186100761865252</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>[ 0.2126317  -0.31504718]</t>
+          <t>[ 0.21263165 -0.31504723]</t>
         </is>
       </c>
     </row>
@@ -982,13 +982,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.7721853018678833</v>
+        <v>0.772185228876031</v>
       </c>
       <c r="E14" t="n">
-        <v>0.03016477551485748</v>
+        <v>0.03016498529027952</v>
       </c>
       <c r="F14" t="n">
-        <v>9.293356106216711</v>
+        <v>9.293349210705664</v>
       </c>
       <c r="G14" t="n">
         <v>15.4943</v>
@@ -997,11 +997,11 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>0.5997919303367504</v>
+        <v>0.5997914853014117</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>[ 0.26785419 -0.09700595]</t>
+          <t>[ 0.26785419 -0.09700592]</t>
         </is>
       </c>
     </row>
@@ -1022,13 +1022,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.5505465875505141</v>
+        <v>0.5505465446083191</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0686855988563593</v>
+        <v>0.06868595729533095</v>
       </c>
       <c r="F15" t="n">
-        <v>7.381506096692615</v>
+        <v>7.381518027880717</v>
       </c>
       <c r="G15" t="n">
         <v>15.4943</v>
@@ -1037,11 +1037,11 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0.4764013925567863</v>
+        <v>0.4764021625940325</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>[ 0.21649302 -0.02877683]</t>
+          <t>[ 0.21649303 -0.02877684]</t>
         </is>
       </c>
     </row>
@@ -1062,13 +1062,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.6020398630407148</v>
+        <v>0.6020397476619385</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0631437496157131</v>
+        <v>0.06314370940112339</v>
       </c>
       <c r="F16" t="n">
-        <v>8.524155079169752</v>
+        <v>8.524170068501276</v>
       </c>
       <c r="G16" t="n">
         <v>15.4943</v>
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.5501478013959812</v>
+        <v>0.5501487688053849</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1102,13 +1102,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.3725246422785028</v>
+        <v>0.3725246591215406</v>
       </c>
       <c r="E17" t="n">
-        <v>0.08313837459882889</v>
+        <v>0.08313840402119654</v>
       </c>
       <c r="F17" t="n">
-        <v>7.319725762113397</v>
+        <v>7.319725145562557</v>
       </c>
       <c r="G17" t="n">
         <v>15.4943</v>
@@ -1117,11 +1117,11 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>0.4724140982240822</v>
+        <v>0.4724140584319754</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>[ 0.19751083 -0.01785914]</t>
+          <t>[ 0.19751082 -0.01785914]</t>
         </is>
       </c>
     </row>
@@ -1142,13 +1142,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.7658830705050073</v>
+        <v>0.7658831334318821</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01911828951625773</v>
+        <v>0.01911849081782102</v>
       </c>
       <c r="F18" t="n">
-        <v>15.74095588352838</v>
+        <v>15.74098723456522</v>
       </c>
       <c r="G18" t="n">
         <v>15.4943</v>
@@ -1157,11 +1157,11 @@
         <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>1.015919136942513</v>
+        <v>1.015921160334137</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>[ 0.18011771 -0.06764063]</t>
+          <t>[ 0.18011774 -0.06764064]</t>
         </is>
       </c>
     </row>
@@ -1182,13 +1182,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.6021386179596223</v>
+        <v>0.6021386100779408</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0008485689004768245</v>
+        <v>0.0008485706930041688</v>
       </c>
       <c r="F19" t="n">
-        <v>18.15947727430979</v>
+        <v>18.15952315501167</v>
       </c>
       <c r="G19" t="n">
         <v>15.4943</v>
@@ -1197,11 +1197,11 @@
         <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>1.17201017627836</v>
+        <v>1.172013137412576</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>[ 0.55961217 -0.06370079]</t>
+          <t>[ 0.55961215 -0.06370079]</t>
         </is>
       </c>
     </row>
@@ -1222,13 +1222,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.6099211632949364</v>
+        <v>0.6099209620270115</v>
       </c>
       <c r="E20" t="n">
-        <v>0.002027452177843329</v>
+        <v>0.00202742775725777</v>
       </c>
       <c r="F20" t="n">
-        <v>17.59091876843787</v>
+        <v>17.59093869546037</v>
       </c>
       <c r="G20" t="n">
         <v>15.4943</v>
@@ -1237,11 +1237,11 @@
         <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>1.135315488175514</v>
+        <v>1.135316774262817</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>[ 0.47875303 -0.20064189]</t>
+          <t>[ 0.47875293 -0.20064185]</t>
         </is>
       </c>
     </row>
@@ -1262,13 +1262,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.4275101408568411</v>
+        <v>0.4275101007180105</v>
       </c>
       <c r="E21" t="n">
-        <v>0.03383156531121734</v>
+        <v>0.03383070218535345</v>
       </c>
       <c r="F21" t="n">
-        <v>10.48519306123329</v>
+        <v>10.48518143524562</v>
       </c>
       <c r="G21" t="n">
         <v>15.4943</v>
@@ -1277,11 +1277,11 @@
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0.6767129241871717</v>
+        <v>0.6767121738475191</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>[ 0.36061123 -0.50433333]</t>
+          <t>[ 0.36061115 -0.50433351]</t>
         </is>
       </c>
     </row>
@@ -1302,13 +1302,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.5978225160495485</v>
+        <v>0.5978223617730578</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01126702359254859</v>
+        <v>0.01126703751299983</v>
       </c>
       <c r="F22" t="n">
-        <v>12.38660744062619</v>
+        <v>12.38659587350982</v>
       </c>
       <c r="G22" t="n">
         <v>15.4943</v>
@@ -1317,11 +1317,11 @@
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>0.799429947827665</v>
+        <v>0.7994292012875585</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>[ 0.4710037  -0.18720619]</t>
+          <t>[ 0.4710036  -0.18720615]</t>
         </is>
       </c>
     </row>
@@ -1342,13 +1342,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.6269288243491759</v>
+        <v>0.6269290030932835</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2750023459548397</v>
+        <v>0.2750046805800044</v>
       </c>
       <c r="F23" t="n">
-        <v>7.097655564617231</v>
+        <v>7.097662131966908</v>
       </c>
       <c r="G23" t="n">
         <v>15.4943</v>
@@ -1357,11 +1357,11 @@
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0.4580817180909902</v>
+        <v>0.458082141946839</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>[ 0.12747955 -0.40589609]</t>
+          <t>[ 0.12747955 -0.40589612]</t>
         </is>
       </c>
     </row>
@@ -1382,13 +1382,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.6420917582793985</v>
+        <v>0.6420917296715405</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1013521746878666</v>
+        <v>0.1013514275555494</v>
       </c>
       <c r="F24" t="n">
-        <v>7.81891255800633</v>
+        <v>7.818924508511154</v>
       </c>
       <c r="G24" t="n">
         <v>15.4943</v>
@@ -1397,11 +1397,11 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>0.5046315456655887</v>
+        <v>0.5046323169495333</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>[ 0.1408865  -0.12248264]</t>
+          <t>[ 0.1408866  -0.12248282]</t>
         </is>
       </c>
     </row>
@@ -1422,13 +1422,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.6850898890537228</v>
+        <v>0.6850899204272667</v>
       </c>
       <c r="E25" t="n">
-        <v>0.001150513855321031</v>
+        <v>0.001150516603473799</v>
       </c>
       <c r="F25" t="n">
-        <v>16.78220018378531</v>
+        <v>16.78219035559083</v>
       </c>
       <c r="G25" t="n">
         <v>15.4943</v>
@@ -1437,11 +1437,11 @@
         <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>1.083120901478951</v>
+        <v>1.083120267168626</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>[ 0.7632276  -0.22079367]</t>
+          <t>[ 0.76322768 -0.22079373]</t>
         </is>
       </c>
     </row>
@@ -1462,13 +1462,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.703761072875736</v>
+        <v>0.7037610421524042</v>
       </c>
       <c r="E26" t="n">
-        <v>0.002482864907776305</v>
+        <v>0.00248283298082216</v>
       </c>
       <c r="F26" t="n">
-        <v>17.44921113920149</v>
+        <v>17.44924399721732</v>
       </c>
       <c r="G26" t="n">
         <v>15.4943</v>
@@ -1477,11 +1477,11 @@
         <v>1</v>
       </c>
       <c r="I26" t="n">
-        <v>1.126169697191967</v>
+        <v>1.126171817843808</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>[ 0.60993769 -0.71030695]</t>
+          <t>[ 0.60993771 -0.71030696]</t>
         </is>
       </c>
     </row>
@@ -1502,13 +1502,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.6463059403572415</v>
+        <v>0.6463059737201324</v>
       </c>
       <c r="E27" t="n">
-        <v>0.003636998589662188</v>
+        <v>0.003636994000681314</v>
       </c>
       <c r="F27" t="n">
-        <v>15.61973390592196</v>
+        <v>15.61975608935025</v>
       </c>
       <c r="G27" t="n">
         <v>15.4943</v>
@@ -1517,7 +1517,7 @@
         <v>1</v>
       </c>
       <c r="I27" t="n">
-        <v>1.00809548710958</v>
+        <v>1.008096918825003</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>

</xml_diff>